<commit_message>
like and unlike buttons
like and unlike buttons
</commit_message>
<xml_diff>
--- a/JS-Frameworks-Self-Evaluation-Protocol.xlsx
+++ b/JS-Frameworks-Self-Evaluation-Protocol.xlsx
@@ -739,7 +739,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>18</v>
@@ -1140,7 +1140,7 @@
       </c>
       <c r="C44" s="11">
         <f>SUM(C6:C43)</f>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D44" s="11">
         <v>370</v>

</xml_diff>